<commit_message>
Updated till section 25
</commit_message>
<xml_diff>
--- a/Excel103-AdvancedExercises.xlsx
+++ b/Excel103-AdvancedExercises.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
   <workbookPr codeName="ThisWorkbook" checkCompatibility="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Excel-Udemy\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Excel Practice\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F304C110-FB11-4BA8-8DF6-8F67D36592A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DDBA9A3-1573-4BBA-9286-E0232086D958}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="IF Function" sheetId="4" r:id="rId1"/>
@@ -105,7 +105,10 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -1964,13 +1967,13 @@
     <xf numFmtId="0" fontId="16" fillId="8" borderId="17" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="8" borderId="3" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2673,21 +2676,21 @@
       <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultRowHeight="12.5"/>
   <cols>
-    <col min="1" max="1" width="15.5546875" customWidth="1"/>
-    <col min="2" max="2" width="11.33203125" customWidth="1"/>
-    <col min="3" max="3" width="11.5546875" customWidth="1"/>
-    <col min="4" max="4" width="11.88671875" customWidth="1"/>
-    <col min="5" max="5" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.33203125" customWidth="1"/>
-    <col min="7" max="7" width="1.109375" customWidth="1"/>
-    <col min="8" max="8" width="20.109375" customWidth="1"/>
-    <col min="9" max="9" width="15.88671875" customWidth="1"/>
+    <col min="1" max="1" width="15.54296875" customWidth="1"/>
+    <col min="2" max="2" width="11.36328125" customWidth="1"/>
+    <col min="3" max="3" width="11.54296875" customWidth="1"/>
+    <col min="4" max="4" width="11.90625" customWidth="1"/>
+    <col min="5" max="5" width="11.6328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.36328125" customWidth="1"/>
+    <col min="7" max="7" width="1.08984375" customWidth="1"/>
+    <col min="8" max="8" width="20.08984375" customWidth="1"/>
+    <col min="9" max="9" width="15.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="13.8" thickBot="1"/>
-    <row r="2" spans="1:9" ht="16.2" thickBot="1">
+    <row r="1" spans="1:9" ht="13" thickBot="1"/>
+    <row r="2" spans="1:9" ht="16" thickBot="1">
       <c r="A2" s="129" t="s">
         <v>280</v>
       </c>
@@ -2703,8 +2706,8 @@
         <v>34000</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="14.4" thickTop="1" thickBot="1"/>
-    <row r="4" spans="1:9" ht="13.8">
+    <row r="3" spans="1:9" ht="13.5" thickTop="1" thickBot="1"/>
+    <row r="4" spans="1:9" ht="14">
       <c r="A4" s="41" t="s">
         <v>1</v>
       </c>
@@ -2730,7 +2733,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="15.6">
+    <row r="5" spans="1:9" ht="15.5">
       <c r="A5" s="5" t="s">
         <v>9</v>
       </c>
@@ -2759,7 +2762,7 @@
         <v>BONUS</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="15.6">
+    <row r="6" spans="1:9" ht="15.5">
       <c r="A6" s="5" t="s">
         <v>10</v>
       </c>
@@ -2784,11 +2787,11 @@
         <v>NO</v>
       </c>
       <c r="I6" s="2" t="str">
-        <f t="shared" ref="I6:I9" si="0">IF(AND(H6 = "YES",MIN(B6:E6) &gt;= 8000),"BONUS","NO BONUS")</f>
+        <f t="shared" ref="I6:I8" si="0">IF(AND(H6 = "YES",MIN(B6:E6) &gt;= 8000),"BONUS","NO BONUS")</f>
         <v>NO BONUS</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="15.6">
+    <row r="7" spans="1:9" ht="15.5">
       <c r="A7" s="5" t="s">
         <v>11</v>
       </c>
@@ -2817,7 +2820,7 @@
         <v>NO BONUS</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="15.6">
+    <row r="8" spans="1:9" ht="15.5">
       <c r="A8" s="5" t="s">
         <v>15</v>
       </c>
@@ -2846,7 +2849,7 @@
         <v>BONUS</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="16.2" thickBot="1">
+    <row r="9" spans="1:9" ht="16" thickBot="1">
       <c r="A9" s="16" t="s">
         <v>14</v>
       </c>
@@ -2875,7 +2878,7 @@
         <v>NO BONUS</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="13.8">
+    <row r="10" spans="1:9" ht="14">
       <c r="A10" s="48" t="s">
         <v>223</v>
       </c>
@@ -2891,7 +2894,7 @@
       <c r="E10" s="54"/>
       <c r="F10" s="54"/>
     </row>
-    <row r="11" spans="1:9" s="50" customFormat="1" ht="13.8">
+    <row r="11" spans="1:9" s="50" customFormat="1" ht="14">
       <c r="A11" s="49"/>
     </row>
     <row r="12" spans="1:9" ht="16.5" customHeight="1">
@@ -2928,14 +2931,14 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultRowHeight="12.5"/>
   <cols>
-    <col min="1" max="1" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.08984375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.6">
+    <row r="1" spans="1:3" ht="15.5">
       <c r="A1" s="72" t="s">
         <v>242</v>
       </c>
@@ -2986,198 +2989,191 @@
       <selection activeCell="E4" sqref="E4:F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultRowHeight="12.5"/>
   <cols>
-    <col min="2" max="2" width="12.88671875" customWidth="1"/>
-    <col min="3" max="3" width="12.109375" customWidth="1"/>
-    <col min="4" max="4" width="3.109375" customWidth="1"/>
-    <col min="6" max="6" width="15.44140625" customWidth="1"/>
+    <col min="2" max="2" width="12.90625" customWidth="1"/>
+    <col min="3" max="3" width="12.08984375" customWidth="1"/>
+    <col min="4" max="4" width="3.08984375" customWidth="1"/>
+    <col min="6" max="6" width="15.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6">
+    <row r="2" spans="2:6" ht="13">
       <c r="B2" s="40" t="s">
         <v>17</v>
       </c>
       <c r="C2" s="40" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="132" t="s">
+      <c r="E2" s="134" t="s">
         <v>166</v>
       </c>
-      <c r="F2" s="132"/>
-    </row>
-    <row r="3" spans="2:6">
+      <c r="F2" s="134"/>
+    </row>
+    <row r="3" spans="2:6" ht="13">
       <c r="B3" s="25" t="s">
         <v>25</v>
       </c>
       <c r="C3" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="E3" s="133" t="str">
+      <c r="E3" s="132" t="str">
         <f>CONCATENATE(C3," ",B3)</f>
         <v>Howard Smith</v>
       </c>
-      <c r="F3" s="134"/>
-    </row>
-    <row r="4" spans="2:6">
+      <c r="F3" s="133"/>
+    </row>
+    <row r="4" spans="2:6" ht="13">
       <c r="B4" s="25" t="s">
         <v>30</v>
       </c>
       <c r="C4" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="E4" s="133"/>
-      <c r="F4" s="134"/>
-    </row>
-    <row r="5" spans="2:6">
+      <c r="E4" s="132"/>
+      <c r="F4" s="133"/>
+    </row>
+    <row r="5" spans="2:6" ht="13">
       <c r="B5" s="25" t="s">
         <v>33</v>
       </c>
       <c r="C5" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="E5" s="133"/>
-      <c r="F5" s="134"/>
-    </row>
-    <row r="6" spans="2:6">
+      <c r="E5" s="132"/>
+      <c r="F5" s="133"/>
+    </row>
+    <row r="6" spans="2:6" ht="13">
       <c r="B6" s="25" t="s">
         <v>36</v>
       </c>
       <c r="C6" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="E6" s="133"/>
-      <c r="F6" s="134"/>
-    </row>
-    <row r="7" spans="2:6">
+      <c r="E6" s="132"/>
+      <c r="F6" s="133"/>
+    </row>
+    <row r="7" spans="2:6" ht="13">
       <c r="B7" s="25" t="s">
         <v>41</v>
       </c>
       <c r="C7" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="E7" s="133"/>
-      <c r="F7" s="134"/>
-    </row>
-    <row r="8" spans="2:6">
+      <c r="E7" s="132"/>
+      <c r="F7" s="133"/>
+    </row>
+    <row r="8" spans="2:6" ht="13">
       <c r="B8" s="25" t="s">
         <v>45</v>
       </c>
       <c r="C8" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="E8" s="133"/>
-      <c r="F8" s="134"/>
-    </row>
-    <row r="9" spans="2:6">
+      <c r="E8" s="132"/>
+      <c r="F8" s="133"/>
+    </row>
+    <row r="9" spans="2:6" ht="13">
       <c r="B9" s="25" t="s">
         <v>48</v>
       </c>
       <c r="C9" s="25" t="s">
         <v>49</v>
       </c>
-      <c r="E9" s="133"/>
-      <c r="F9" s="134"/>
-    </row>
-    <row r="10" spans="2:6">
+      <c r="E9" s="132"/>
+      <c r="F9" s="133"/>
+    </row>
+    <row r="10" spans="2:6" ht="13">
       <c r="B10" s="25" t="s">
         <v>52</v>
       </c>
       <c r="C10" s="25" t="s">
         <v>53</v>
       </c>
-      <c r="E10" s="133"/>
-      <c r="F10" s="134"/>
-    </row>
-    <row r="11" spans="2:6">
+      <c r="E10" s="132"/>
+      <c r="F10" s="133"/>
+    </row>
+    <row r="11" spans="2:6" ht="13">
       <c r="B11" s="25" t="s">
         <v>56</v>
       </c>
       <c r="C11" s="25" t="s">
         <v>57</v>
       </c>
-      <c r="E11" s="133"/>
-      <c r="F11" s="134"/>
-    </row>
-    <row r="12" spans="2:6">
+      <c r="E11" s="132"/>
+      <c r="F11" s="133"/>
+    </row>
+    <row r="12" spans="2:6" ht="13">
       <c r="B12" s="25" t="s">
         <v>59</v>
       </c>
       <c r="C12" s="25" t="s">
         <v>60</v>
       </c>
-      <c r="E12" s="133"/>
-      <c r="F12" s="134"/>
-    </row>
-    <row r="13" spans="2:6">
+      <c r="E12" s="132"/>
+      <c r="F12" s="133"/>
+    </row>
+    <row r="13" spans="2:6" ht="13">
       <c r="B13" s="25" t="s">
         <v>62</v>
       </c>
       <c r="C13" s="25" t="s">
         <v>63</v>
       </c>
-      <c r="E13" s="133"/>
-      <c r="F13" s="134"/>
-    </row>
-    <row r="14" spans="2:6">
+      <c r="E13" s="132"/>
+      <c r="F13" s="133"/>
+    </row>
+    <row r="14" spans="2:6" ht="13">
       <c r="B14" s="25" t="s">
         <v>66</v>
       </c>
       <c r="C14" s="25" t="s">
         <v>67</v>
       </c>
-      <c r="E14" s="133"/>
-      <c r="F14" s="134"/>
-    </row>
-    <row r="15" spans="2:6">
+      <c r="E14" s="132"/>
+      <c r="F14" s="133"/>
+    </row>
+    <row r="15" spans="2:6" ht="13">
       <c r="B15" s="25" t="s">
         <v>25</v>
       </c>
       <c r="C15" s="25" t="s">
         <v>69</v>
       </c>
-      <c r="E15" s="133"/>
-      <c r="F15" s="134"/>
-    </row>
-    <row r="16" spans="2:6">
+      <c r="E15" s="132"/>
+      <c r="F15" s="133"/>
+    </row>
+    <row r="16" spans="2:6" ht="13">
       <c r="B16" s="25" t="s">
         <v>71</v>
       </c>
       <c r="C16" s="25" t="s">
         <v>72</v>
       </c>
-      <c r="E16" s="133"/>
-      <c r="F16" s="134"/>
-    </row>
-    <row r="17" spans="2:6">
+      <c r="E16" s="132"/>
+      <c r="F16" s="133"/>
+    </row>
+    <row r="17" spans="2:6" ht="13">
       <c r="B17" s="25" t="s">
         <v>74</v>
       </c>
       <c r="C17" s="25" t="s">
         <v>75</v>
       </c>
-      <c r="E17" s="133"/>
-      <c r="F17" s="134"/>
-    </row>
-    <row r="18" spans="2:6">
+      <c r="E17" s="132"/>
+      <c r="F17" s="133"/>
+    </row>
+    <row r="18" spans="2:6" ht="13">
       <c r="B18" s="25" t="s">
         <v>77</v>
       </c>
       <c r="C18" s="25" t="s">
         <v>78</v>
       </c>
-      <c r="E18" s="133"/>
-      <c r="F18" s="134"/>
+      <c r="E18" s="132"/>
+      <c r="F18" s="133"/>
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="E17:F17"/>
     <mergeCell ref="E2:F2"/>
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="E4:F4"/>
@@ -3188,6 +3184,13 @@
     <mergeCell ref="E6:F6"/>
     <mergeCell ref="E7:F7"/>
     <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="E17:F17"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3204,21 +3207,21 @@
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultRowHeight="12.5"/>
   <cols>
-    <col min="1" max="1" width="15.5546875" customWidth="1"/>
-    <col min="2" max="2" width="11.33203125" customWidth="1"/>
-    <col min="3" max="3" width="11.5546875" customWidth="1"/>
-    <col min="4" max="4" width="11.88671875" customWidth="1"/>
-    <col min="5" max="5" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.33203125" customWidth="1"/>
-    <col min="7" max="7" width="1.109375" customWidth="1"/>
-    <col min="8" max="8" width="20.109375" customWidth="1"/>
-    <col min="9" max="9" width="15.88671875" customWidth="1"/>
+    <col min="1" max="1" width="15.54296875" customWidth="1"/>
+    <col min="2" max="2" width="11.36328125" customWidth="1"/>
+    <col min="3" max="3" width="11.54296875" customWidth="1"/>
+    <col min="4" max="4" width="11.90625" customWidth="1"/>
+    <col min="5" max="5" width="11.6328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.36328125" customWidth="1"/>
+    <col min="7" max="7" width="1.08984375" customWidth="1"/>
+    <col min="8" max="8" width="20.08984375" customWidth="1"/>
+    <col min="9" max="9" width="15.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="13.8" thickBot="1"/>
-    <row r="2" spans="1:9" ht="16.2" thickBot="1">
+    <row r="1" spans="1:9" ht="13" thickBot="1"/>
+    <row r="2" spans="1:9" ht="16" thickBot="1">
       <c r="A2" s="129" t="s">
         <v>222</v>
       </c>
@@ -3234,8 +3237,8 @@
         <v>34000</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="14.4" thickTop="1" thickBot="1"/>
-    <row r="4" spans="1:9" ht="13.8">
+    <row r="3" spans="1:9" ht="13.5" thickTop="1" thickBot="1"/>
+    <row r="4" spans="1:9" ht="14">
       <c r="A4" s="41" t="s">
         <v>1</v>
       </c>
@@ -3261,7 +3264,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="15.6">
+    <row r="5" spans="1:9" ht="15.5">
       <c r="A5" s="5" t="s">
         <v>9</v>
       </c>
@@ -3290,7 +3293,7 @@
         <v>BONUS</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="15.6">
+    <row r="6" spans="1:9" ht="15.5">
       <c r="A6" s="5" t="s">
         <v>10</v>
       </c>
@@ -3319,7 +3322,7 @@
         <v>NO BONUS</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="15.6">
+    <row r="7" spans="1:9" ht="15.5">
       <c r="A7" s="5" t="s">
         <v>11</v>
       </c>
@@ -3348,7 +3351,7 @@
         <v>NO BONUS</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="15.6">
+    <row r="8" spans="1:9" ht="15.5">
       <c r="A8" s="5" t="s">
         <v>15</v>
       </c>
@@ -3377,7 +3380,7 @@
         <v>BONUS</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="16.2" thickBot="1">
+    <row r="9" spans="1:9" ht="16" thickBot="1">
       <c r="A9" s="16" t="s">
         <v>14</v>
       </c>
@@ -3406,7 +3409,7 @@
         <v>NO BONUS</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="13.8">
+    <row r="10" spans="1:9" ht="14">
       <c r="A10" s="48" t="s">
         <v>223</v>
       </c>
@@ -3431,7 +3434,7 @@
         <v>176211</v>
       </c>
     </row>
-    <row r="11" spans="1:9" s="50" customFormat="1" ht="13.8">
+    <row r="11" spans="1:9" s="50" customFormat="1" ht="14">
       <c r="A11" s="49"/>
     </row>
     <row r="12" spans="1:9" ht="15.75" customHeight="1">
@@ -3477,13 +3480,13 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultRowHeight="12.5"/>
   <cols>
-    <col min="1" max="1" width="20.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.36328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" ht="13">
       <c r="A2" s="71" t="s">
         <v>249</v>
       </c>
@@ -3506,21 +3509,21 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultRowHeight="12.5"/>
   <cols>
-    <col min="1" max="1" width="15.5546875" customWidth="1"/>
-    <col min="2" max="2" width="11.33203125" customWidth="1"/>
-    <col min="3" max="3" width="11.5546875" customWidth="1"/>
-    <col min="4" max="4" width="11.88671875" customWidth="1"/>
-    <col min="5" max="5" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.33203125" customWidth="1"/>
-    <col min="7" max="7" width="1.109375" customWidth="1"/>
-    <col min="8" max="8" width="20.109375" customWidth="1"/>
-    <col min="9" max="9" width="15.88671875" customWidth="1"/>
+    <col min="1" max="1" width="15.54296875" customWidth="1"/>
+    <col min="2" max="2" width="11.36328125" customWidth="1"/>
+    <col min="3" max="3" width="11.54296875" customWidth="1"/>
+    <col min="4" max="4" width="11.90625" customWidth="1"/>
+    <col min="5" max="5" width="11.6328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.36328125" customWidth="1"/>
+    <col min="7" max="7" width="1.08984375" customWidth="1"/>
+    <col min="8" max="8" width="20.08984375" customWidth="1"/>
+    <col min="9" max="9" width="15.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="13.8" thickBot="1"/>
-    <row r="2" spans="1:9" ht="16.2" thickBot="1">
+    <row r="1" spans="1:9" ht="13" thickBot="1"/>
+    <row r="2" spans="1:9" ht="16" thickBot="1">
       <c r="A2" s="129" t="s">
         <v>222</v>
       </c>
@@ -3536,8 +3539,8 @@
         <v>34000</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="14.4" thickTop="1" thickBot="1"/>
-    <row r="4" spans="1:9" ht="13.8">
+    <row r="3" spans="1:9" ht="13.5" thickTop="1" thickBot="1"/>
+    <row r="4" spans="1:9" ht="14">
       <c r="A4" s="41" t="s">
         <v>1</v>
       </c>
@@ -3563,7 +3566,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="15.6">
+    <row r="5" spans="1:9" ht="15.5">
       <c r="A5" s="5" t="s">
         <v>9</v>
       </c>
@@ -3592,7 +3595,7 @@
         <v>BONUS</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="15.6">
+    <row r="6" spans="1:9" ht="15.5">
       <c r="A6" s="5" t="s">
         <v>10</v>
       </c>
@@ -3621,7 +3624,7 @@
         <v>NO BONUS</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="15.6">
+    <row r="7" spans="1:9" ht="15.5">
       <c r="A7" s="5" t="s">
         <v>11</v>
       </c>
@@ -3650,7 +3653,7 @@
         <v>NO BONUS</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="15.6">
+    <row r="8" spans="1:9" ht="15.5">
       <c r="A8" s="5" t="s">
         <v>15</v>
       </c>
@@ -3679,7 +3682,7 @@
         <v>BONUS</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="16.2" thickBot="1">
+    <row r="9" spans="1:9" ht="16" thickBot="1">
       <c r="A9" s="16" t="s">
         <v>14</v>
       </c>
@@ -3708,7 +3711,7 @@
         <v>NO BONUS</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="13.8">
+    <row r="10" spans="1:9" ht="14">
       <c r="A10" s="48" t="s">
         <v>223</v>
       </c>
@@ -3733,7 +3736,7 @@
         <v>176211</v>
       </c>
     </row>
-    <row r="11" spans="1:9" s="50" customFormat="1" ht="13.8">
+    <row r="11" spans="1:9" s="50" customFormat="1" ht="14">
       <c r="A11" s="49"/>
     </row>
     <row r="12" spans="1:9" ht="15.75" customHeight="1">
@@ -3780,15 +3783,15 @@
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultRowHeight="12.5"/>
   <cols>
     <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="13.8" thickBot="1"/>
-    <row r="2" spans="1:4">
+    <row r="1" spans="1:4" ht="13" thickBot="1"/>
+    <row r="2" spans="1:4" ht="13">
       <c r="A2" s="98" t="s">
         <v>254</v>
       </c>
@@ -3800,7 +3803,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="13.8" thickBot="1">
+    <row r="3" spans="1:4" ht="13.5" thickBot="1">
       <c r="A3" s="98" t="s">
         <v>252</v>
       </c>
@@ -3810,7 +3813,7 @@
       <c r="C3" s="75"/>
       <c r="D3" s="96"/>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" ht="13">
       <c r="A4" s="98" t="s">
         <v>251</v>
       </c>
@@ -3834,17 +3837,17 @@
       <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="12.5"/>
   <cols>
-    <col min="1" max="1" width="25.44140625" style="79" customWidth="1"/>
-    <col min="2" max="2" width="10.109375" style="79" customWidth="1"/>
-    <col min="3" max="3" width="10.5546875" style="79" customWidth="1"/>
-    <col min="4" max="4" width="10.33203125" style="79" customWidth="1"/>
-    <col min="5" max="5" width="9.33203125" style="79" customWidth="1"/>
-    <col min="6" max="6" width="8.88671875" style="79" customWidth="1"/>
-    <col min="7" max="7" width="11.33203125" style="79" customWidth="1"/>
-    <col min="8" max="8" width="15.6640625" style="79" customWidth="1"/>
-    <col min="9" max="16384" width="9.109375" style="79"/>
+    <col min="1" max="1" width="25.453125" style="79" customWidth="1"/>
+    <col min="2" max="2" width="10.08984375" style="79" customWidth="1"/>
+    <col min="3" max="3" width="10.54296875" style="79" customWidth="1"/>
+    <col min="4" max="4" width="10.36328125" style="79" customWidth="1"/>
+    <col min="5" max="5" width="9.36328125" style="79" customWidth="1"/>
+    <col min="6" max="6" width="8.90625" style="79" customWidth="1"/>
+    <col min="7" max="7" width="11.36328125" style="79" customWidth="1"/>
+    <col min="8" max="8" width="15.6328125" style="79" customWidth="1"/>
+    <col min="9" max="16384" width="9.08984375" style="79"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="10.5" customHeight="1">
@@ -3865,7 +3868,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="16.2" thickBot="1">
+    <row r="4" spans="1:8" ht="16" thickBot="1">
       <c r="A4" s="90" t="s">
         <v>278</v>
       </c>
@@ -3889,7 +3892,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="15.6">
+    <row r="5" spans="1:8" ht="15.5">
       <c r="A5" s="88" t="s">
         <v>271</v>
       </c>
@@ -3914,7 +3917,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="15.6">
+    <row r="6" spans="1:8" ht="15.5">
       <c r="A6" s="88" t="s">
         <v>270</v>
       </c>
@@ -3939,7 +3942,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="15.6">
+    <row r="7" spans="1:8" ht="15.5">
       <c r="A7" s="88" t="s">
         <v>269</v>
       </c>
@@ -3964,7 +3967,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="15.6">
+    <row r="8" spans="1:8" ht="15.5">
       <c r="A8" s="99" t="s">
         <v>268</v>
       </c>
@@ -3999,7 +4002,7 @@
       <c r="E9" s="81"/>
       <c r="F9" s="75"/>
     </row>
-    <row r="10" spans="1:8" ht="15.6">
+    <row r="10" spans="1:8" ht="15.5">
       <c r="A10" s="100" t="s">
         <v>267</v>
       </c>
@@ -4017,7 +4020,7 @@
       </c>
       <c r="F10" s="75"/>
     </row>
-    <row r="11" spans="1:8" ht="15.6">
+    <row r="11" spans="1:8" ht="15.5">
       <c r="A11" s="80"/>
       <c r="F11" s="75"/>
     </row>
@@ -4042,15 +4045,15 @@
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="12.5"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="75"/>
-    <col min="2" max="2" width="17.44140625" style="75" bestFit="1" customWidth="1"/>
-    <col min="3" max="6" width="12.44140625" style="75" customWidth="1"/>
-    <col min="7" max="16384" width="9.109375" style="75"/>
+    <col min="1" max="1" width="9.08984375" style="75"/>
+    <col min="2" max="2" width="17.453125" style="75" bestFit="1" customWidth="1"/>
+    <col min="3" max="6" width="12.453125" style="75" customWidth="1"/>
+    <col min="7" max="16384" width="9.08984375" style="75"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3">
+    <row r="2" spans="2:3" ht="13">
       <c r="B2" s="98" t="s">
         <v>254</v>
       </c>
@@ -4058,7 +4061,7 @@
         <v>220000</v>
       </c>
     </row>
-    <row r="3" spans="2:3">
+    <row r="3" spans="2:3" ht="13">
       <c r="B3" s="98" t="s">
         <v>252</v>
       </c>
@@ -4066,7 +4069,7 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="4" spans="2:3">
+    <row r="4" spans="2:3" ht="13">
       <c r="B4" s="98" t="s">
         <v>251</v>
       </c>
@@ -4078,7 +4081,7 @@
     <row r="6" spans="2:3">
       <c r="C6" s="77"/>
     </row>
-    <row r="7" spans="2:3" ht="15.6">
+    <row r="7" spans="2:3" ht="15.5">
       <c r="B7" s="112" t="s">
         <v>250</v>
       </c>
@@ -4087,43 +4090,43 @@
         <v>1697.9956826206067</v>
       </c>
     </row>
-    <row r="8" spans="2:3" ht="15.6">
+    <row r="8" spans="2:3" ht="15.5">
       <c r="B8" s="76">
         <v>7.2499999999999995E-2</v>
       </c>
       <c r="C8" s="12"/>
     </row>
-    <row r="9" spans="2:3" ht="15.6">
+    <row r="9" spans="2:3" ht="15.5">
       <c r="B9" s="76">
         <v>7.4999999999999997E-2</v>
       </c>
       <c r="C9" s="12"/>
     </row>
-    <row r="10" spans="2:3" ht="15.6">
+    <row r="10" spans="2:3" ht="15.5">
       <c r="B10" s="76">
         <v>7.7499999999999999E-2</v>
       </c>
       <c r="C10" s="12"/>
     </row>
-    <row r="11" spans="2:3" ht="15.6">
+    <row r="11" spans="2:3" ht="15.5">
       <c r="B11" s="76">
         <v>8.2500000000000004E-2</v>
       </c>
       <c r="C11" s="12"/>
     </row>
-    <row r="12" spans="2:3" ht="15.6">
+    <row r="12" spans="2:3" ht="15.5">
       <c r="B12" s="76">
         <v>8.5000000000000006E-2</v>
       </c>
       <c r="C12" s="12"/>
     </row>
-    <row r="13" spans="2:3" ht="15.6">
+    <row r="13" spans="2:3" ht="15.5">
       <c r="B13" s="76">
         <v>8.7499999999999994E-2</v>
       </c>
       <c r="C13" s="12"/>
     </row>
-    <row r="14" spans="2:3" ht="15.6">
+    <row r="14" spans="2:3" ht="15.5">
       <c r="B14" s="76">
         <v>0.09</v>
       </c>
@@ -4149,16 +4152,16 @@
       <selection activeCell="C11" sqref="C11:C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="12.5"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="75"/>
-    <col min="2" max="2" width="11.5546875" style="75" customWidth="1"/>
-    <col min="3" max="6" width="14.88671875" style="75" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.6640625" style="75" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.109375" style="75"/>
+    <col min="1" max="1" width="9.08984375" style="75"/>
+    <col min="2" max="2" width="11.54296875" style="75" customWidth="1"/>
+    <col min="3" max="6" width="14.90625" style="75" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.6328125" style="75" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.08984375" style="75"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7" ht="15.6">
+    <row r="2" spans="2:7" ht="15.5">
       <c r="B2" s="112" t="s">
         <v>266</v>
       </c>
@@ -4178,7 +4181,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="3" spans="2:7">
+    <row r="3" spans="2:7" ht="13">
       <c r="B3" s="113" t="s">
         <v>258</v>
       </c>
@@ -4202,7 +4205,7 @@
         <v>358431.46368858824</v>
       </c>
     </row>
-    <row r="4" spans="2:7">
+    <row r="4" spans="2:7" ht="13">
       <c r="B4" s="113" t="s">
         <v>257</v>
       </c>
@@ -4226,7 +4229,7 @@
         <v>314199.50175383873</v>
       </c>
     </row>
-    <row r="5" spans="2:7">
+    <row r="5" spans="2:7" ht="13">
       <c r="B5" s="113" t="s">
         <v>256</v>
       </c>
@@ -4250,7 +4253,7 @@
         <v>386317.03597964835</v>
       </c>
     </row>
-    <row r="6" spans="2:7">
+    <row r="6" spans="2:7" ht="13">
       <c r="B6" s="113" t="s">
         <v>255</v>
       </c>
@@ -4274,7 +4277,7 @@
         <v>267970.20047823974</v>
       </c>
     </row>
-    <row r="7" spans="2:7" ht="15.6">
+    <row r="7" spans="2:7" ht="15.5">
       <c r="B7" s="101" t="s">
         <v>260</v>
       </c>
@@ -4299,13 +4302,13 @@
         <v>1326918.201900315</v>
       </c>
     </row>
-    <row r="10" spans="2:7">
+    <row r="10" spans="2:7" ht="13">
       <c r="B10" s="135" t="s">
         <v>259</v>
       </c>
       <c r="C10" s="135"/>
     </row>
-    <row r="11" spans="2:7">
+    <row r="11" spans="2:7" ht="13">
       <c r="B11" s="115" t="s">
         <v>258</v>
       </c>
@@ -4313,7 +4316,7 @@
         <v>3.3000000000000002E-2</v>
       </c>
     </row>
-    <row r="12" spans="2:7">
+    <row r="12" spans="2:7" ht="13">
       <c r="B12" s="115" t="s">
         <v>257</v>
       </c>
@@ -4321,7 +4324,7 @@
         <v>2.3E-2</v>
       </c>
     </row>
-    <row r="13" spans="2:7">
+    <row r="13" spans="2:7" ht="13">
       <c r="B13" s="115" t="s">
         <v>256</v>
       </c>
@@ -4329,7 +4332,7 @@
         <v>4.2999999999999997E-2</v>
       </c>
     </row>
-    <row r="14" spans="2:7">
+    <row r="14" spans="2:7" ht="13">
       <c r="B14" s="115" t="s">
         <v>255</v>
       </c>
@@ -4358,13 +4361,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultRowHeight="12.5"/>
   <cols>
-    <col min="2" max="2" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.6640625" customWidth="1"/>
-    <col min="8" max="8" width="13.109375" style="119" customWidth="1"/>
-    <col min="9" max="9" width="9.109375" style="117"/>
+    <col min="2" max="2" width="11.08984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.90625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.6328125" customWidth="1"/>
+    <col min="8" max="8" width="13.08984375" style="119" customWidth="1"/>
+    <col min="9" max="9" width="9.08984375" style="117"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -4976,7 +4979,7 @@
         <v>11.9</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="26.4">
+    <row r="22" spans="1:9">
       <c r="A22" s="7">
         <v>1673</v>
       </c>
@@ -5454,20 +5457,20 @@
       <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="12.5"/>
   <cols>
-    <col min="1" max="1" width="13.33203125" style="18" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.5546875" style="18" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.36328125" style="18" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.54296875" style="18" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" style="18" customWidth="1"/>
-    <col min="4" max="4" width="12.5546875" style="18" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.109375" style="18" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.109375" style="18"/>
-    <col min="7" max="7" width="13.6640625" style="18" customWidth="1"/>
-    <col min="8" max="9" width="12.6640625" style="18" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="9.109375" style="18"/>
+    <col min="4" max="4" width="12.54296875" style="18" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.08984375" style="18" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.08984375" style="18"/>
+    <col min="7" max="7" width="13.6328125" style="18" customWidth="1"/>
+    <col min="8" max="9" width="12.6328125" style="18" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.08984375" style="18"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:9" ht="15.6">
+    <row r="2" spans="1:9" ht="15.5">
       <c r="A2" s="29" t="s">
         <v>143</v>
       </c>
@@ -5493,7 +5496,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="15.6">
+    <row r="3" spans="1:9" ht="15.5">
       <c r="A3" s="19" t="s">
         <v>145</v>
       </c>
@@ -5522,7 +5525,7 @@
         <v>491064</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" ht="13">
       <c r="A4" s="19" t="s">
         <v>145</v>
       </c>
@@ -5549,7 +5552,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="15.6">
+    <row r="5" spans="1:9" ht="15.5">
       <c r="A5" s="19" t="s">
         <v>145</v>
       </c>
@@ -10399,13 +10402,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultRowHeight="12.5"/>
   <cols>
-    <col min="2" max="2" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.5546875" style="119" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.109375" style="117"/>
+    <col min="2" max="2" width="11.08984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.90625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.08984375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.54296875" style="119" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.08984375" style="117"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -11017,7 +11020,7 @@
         <v>11.9</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="26.4">
+    <row r="22" spans="1:9">
       <c r="A22" s="7">
         <v>1673</v>
       </c>
@@ -11491,21 +11494,21 @@
   <sheetPr codeName="Sheet10"/>
   <dimension ref="B1:G18"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView showGridLines="0" topLeftCell="A4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultRowHeight="12.5"/>
   <cols>
-    <col min="1" max="1" width="3.44140625" customWidth="1"/>
-    <col min="2" max="2" width="13.88671875" customWidth="1"/>
-    <col min="3" max="3" width="19.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.5546875" customWidth="1"/>
-    <col min="5" max="6" width="13.88671875" customWidth="1"/>
-    <col min="7" max="7" width="3.109375" customWidth="1"/>
+    <col min="1" max="1" width="3.453125" customWidth="1"/>
+    <col min="2" max="2" width="13.90625" customWidth="1"/>
+    <col min="3" max="3" width="19.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.54296875" customWidth="1"/>
+    <col min="5" max="6" width="13.90625" customWidth="1"/>
+    <col min="7" max="7" width="3.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" ht="13.8" thickBot="1"/>
+    <row r="1" spans="2:7" ht="13" thickBot="1"/>
     <row r="2" spans="2:7" ht="21.75" customHeight="1">
       <c r="B2" s="33" t="s">
         <v>16</v>
@@ -11529,12 +11532,21 @@
         <v>1054</v>
       </c>
       <c r="C3" s="11" t="str">
-        <f>IFERROR(VLOOKUP($B3,'Master Emp List'!$A$1:$I$38,3,FALSE), "EMP ID NOT FOUND")</f>
+        <f>INDEX('Master Emp List'!$A$1:$I$38,MATCH($B3,'Master Emp List'!$A$1:$A$38,0),MATCH(C$2,'Master Emp List'!$A$1:$I$1,0))</f>
         <v>Howard</v>
       </c>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
+      <c r="D3" s="11" t="str">
+        <f>INDEX('Master Emp List'!$A$1:$I$38,MATCH($B3,'Master Emp List'!$A$1:$A$38,0),MATCH(D$2,'Master Emp List'!$A$1:$I$1,0))</f>
+        <v>Smith</v>
+      </c>
+      <c r="E3" s="11" t="str">
+        <f>INDEX('Master Emp List'!$A$1:$I$38,MATCH($B3,'Master Emp List'!$A$1:$A$38,0),MATCH(E$2,'Master Emp List'!$A$1:$I$1,0))</f>
+        <v>AT</v>
+      </c>
+      <c r="F3" s="11">
+        <f>INDEX('Master Emp List'!$A$1:$I$38,MATCH($B3,'Master Emp List'!$A$1:$A$38,0),MATCH(F$2,'Master Emp List'!$A$1:$I$1,0))</f>
+        <v>11.25</v>
+      </c>
       <c r="G3" s="68"/>
     </row>
     <row r="4" spans="2:7">
@@ -11542,12 +11554,21 @@
         <v>1056</v>
       </c>
       <c r="C4" s="11" t="str">
-        <f>IFERROR(VLOOKUP($B4,'Master Emp List'!$A$1:$I$38,3,FALSE), "EMP ID NOT FOUND")</f>
+        <f>INDEX('Master Emp List'!$A$1:$I$38,MATCH($B4,'Master Emp List'!$A$1:$A$38,0),MATCH(C$2,'Master Emp List'!$A$1:$I$1,0))</f>
         <v>Joe</v>
       </c>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="11"/>
+      <c r="D4" s="11" t="str">
+        <f>INDEX('Master Emp List'!$A$1:$I$38,MATCH($B4,'Master Emp List'!$A$1:$A$38,0),MATCH(D$2,'Master Emp List'!$A$1:$I$1,0))</f>
+        <v>Gonzales</v>
+      </c>
+      <c r="E4" s="11" t="str">
+        <f>INDEX('Master Emp List'!$A$1:$I$38,MATCH($B4,'Master Emp List'!$A$1:$A$38,0),MATCH(E$2,'Master Emp List'!$A$1:$I$1,0))</f>
+        <v>AT</v>
+      </c>
+      <c r="F4" s="11">
+        <f>INDEX('Master Emp List'!$A$1:$I$38,MATCH($B4,'Master Emp List'!$A$1:$A$38,0),MATCH(F$2,'Master Emp List'!$A$1:$I$1,0))</f>
+        <v>12.25</v>
+      </c>
       <c r="G4" s="68"/>
     </row>
     <row r="5" spans="2:7">
@@ -11555,12 +11576,21 @@
         <v>1067</v>
       </c>
       <c r="C5" s="11" t="str">
-        <f>IFERROR(VLOOKUP($B5,'Master Emp List'!$A$1:$I$38,3,FALSE), "EMP ID NOT FOUND")</f>
+        <f>INDEX('Master Emp List'!$A$1:$I$38,MATCH($B5,'Master Emp List'!$A$1:$A$38,0),MATCH(C$2,'Master Emp List'!$A$1:$I$1,0))</f>
         <v>Gail</v>
       </c>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11"/>
-      <c r="F5" s="11"/>
+      <c r="D5" s="11" t="str">
+        <f>INDEX('Master Emp List'!$A$1:$I$38,MATCH($B5,'Master Emp List'!$A$1:$A$38,0),MATCH(D$2,'Master Emp List'!$A$1:$I$1,0))</f>
+        <v>Scote</v>
+      </c>
+      <c r="E5" s="11" t="str">
+        <f>INDEX('Master Emp List'!$A$1:$I$38,MATCH($B5,'Master Emp List'!$A$1:$A$38,0),MATCH(E$2,'Master Emp List'!$A$1:$I$1,0))</f>
+        <v>AT</v>
+      </c>
+      <c r="F5" s="11">
+        <f>INDEX('Master Emp List'!$A$1:$I$38,MATCH($B5,'Master Emp List'!$A$1:$A$38,0),MATCH(F$2,'Master Emp List'!$A$1:$I$1,0))</f>
+        <v>14.55</v>
+      </c>
       <c r="G5" s="68"/>
     </row>
     <row r="6" spans="2:7">
@@ -11568,12 +11598,21 @@
         <v>1075</v>
       </c>
       <c r="C6" s="11" t="str">
-        <f>IFERROR(VLOOKUP($B6,'Master Emp List'!$A$1:$I$38,3,FALSE), "EMP ID NOT FOUND")</f>
+        <f>INDEX('Master Emp List'!$A$1:$I$38,MATCH($B6,'Master Emp List'!$A$1:$A$38,0),MATCH(C$2,'Master Emp List'!$A$1:$I$1,0))</f>
         <v>Sheryl</v>
       </c>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11"/>
-      <c r="F6" s="11"/>
+      <c r="D6" s="11" t="str">
+        <f>INDEX('Master Emp List'!$A$1:$I$38,MATCH($B6,'Master Emp List'!$A$1:$A$38,0),MATCH(D$2,'Master Emp List'!$A$1:$I$1,0))</f>
+        <v>Kane</v>
+      </c>
+      <c r="E6" s="11" t="str">
+        <f>INDEX('Master Emp List'!$A$1:$I$38,MATCH($B6,'Master Emp List'!$A$1:$A$38,0),MATCH(E$2,'Master Emp List'!$A$1:$I$1,0))</f>
+        <v>AD</v>
+      </c>
+      <c r="F6" s="11">
+        <f>INDEX('Master Emp List'!$A$1:$I$38,MATCH($B6,'Master Emp List'!$A$1:$A$38,0),MATCH(F$2,'Master Emp List'!$A$1:$I$1,0))</f>
+        <v>11.25</v>
+      </c>
       <c r="G6" s="68"/>
     </row>
     <row r="7" spans="2:7">
@@ -11581,12 +11620,21 @@
         <v>1078</v>
       </c>
       <c r="C7" s="11" t="str">
-        <f>IFERROR(VLOOKUP($B7,'Master Emp List'!$A$1:$I$38,3,FALSE), "EMP ID NOT FOUND")</f>
+        <f>INDEX('Master Emp List'!$A$1:$I$38,MATCH($B7,'Master Emp List'!$A$1:$A$38,0),MATCH(C$2,'Master Emp List'!$A$1:$I$1,0))</f>
         <v>Kendrick</v>
       </c>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11"/>
-      <c r="F7" s="11"/>
+      <c r="D7" s="11" t="str">
+        <f>INDEX('Master Emp List'!$A$1:$I$38,MATCH($B7,'Master Emp List'!$A$1:$A$38,0),MATCH(D$2,'Master Emp List'!$A$1:$I$1,0))</f>
+        <v>Hapsbuch</v>
+      </c>
+      <c r="E7" s="11" t="str">
+        <f>INDEX('Master Emp List'!$A$1:$I$38,MATCH($B7,'Master Emp List'!$A$1:$A$38,0),MATCH(E$2,'Master Emp List'!$A$1:$I$1,0))</f>
+        <v>AC</v>
+      </c>
+      <c r="F7" s="11">
+        <f>INDEX('Master Emp List'!$A$1:$I$38,MATCH($B7,'Master Emp List'!$A$1:$A$38,0),MATCH(F$2,'Master Emp List'!$A$1:$I$1,0))</f>
+        <v>10.199999999999999</v>
+      </c>
       <c r="G7" s="68"/>
     </row>
     <row r="8" spans="2:7">
@@ -11594,12 +11642,21 @@
         <v>1152</v>
       </c>
       <c r="C8" s="11" t="str">
-        <f>IFERROR(VLOOKUP($B8,'Master Emp List'!$A$1:$I$38,3,FALSE), "EMP ID NOT FOUND")</f>
+        <f>INDEX('Master Emp List'!$A$1:$I$38,MATCH($B8,'Master Emp List'!$A$1:$A$38,0),MATCH(C$2,'Master Emp List'!$A$1:$I$1,0))</f>
         <v>Mark</v>
       </c>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="11"/>
+      <c r="D8" s="11" t="str">
+        <f>INDEX('Master Emp List'!$A$1:$I$38,MATCH($B8,'Master Emp List'!$A$1:$A$38,0),MATCH(D$2,'Master Emp List'!$A$1:$I$1,0))</f>
+        <v>Henders</v>
+      </c>
+      <c r="E8" s="11" t="str">
+        <f>INDEX('Master Emp List'!$A$1:$I$38,MATCH($B8,'Master Emp List'!$A$1:$A$38,0),MATCH(E$2,'Master Emp List'!$A$1:$I$1,0))</f>
+        <v>AD</v>
+      </c>
+      <c r="F8" s="11">
+        <f>INDEX('Master Emp List'!$A$1:$I$38,MATCH($B8,'Master Emp List'!$A$1:$A$38,0),MATCH(F$2,'Master Emp List'!$A$1:$I$1,0))</f>
+        <v>12.25</v>
+      </c>
       <c r="G8" s="68"/>
     </row>
     <row r="9" spans="2:7">
@@ -11607,12 +11664,21 @@
         <v>1196</v>
       </c>
       <c r="C9" s="11" t="str">
-        <f>IFERROR(VLOOKUP($B9,'Master Emp List'!$A$1:$I$38,3,FALSE), "EMP ID NOT FOUND")</f>
+        <f>INDEX('Master Emp List'!$A$1:$I$38,MATCH($B9,'Master Emp List'!$A$1:$A$38,0),MATCH(C$2,'Master Emp List'!$A$1:$I$1,0))</f>
         <v>Katie</v>
       </c>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
+      <c r="D9" s="11" t="str">
+        <f>INDEX('Master Emp List'!$A$1:$I$38,MATCH($B9,'Master Emp List'!$A$1:$A$38,0),MATCH(D$2,'Master Emp List'!$A$1:$I$1,0))</f>
+        <v>Atherton</v>
+      </c>
+      <c r="E9" s="11" t="str">
+        <f>INDEX('Master Emp List'!$A$1:$I$38,MATCH($B9,'Master Emp List'!$A$1:$A$38,0),MATCH(E$2,'Master Emp List'!$A$1:$I$1,0))</f>
+        <v>HR</v>
+      </c>
+      <c r="F9" s="11">
+        <f>INDEX('Master Emp List'!$A$1:$I$38,MATCH($B9,'Master Emp List'!$A$1:$A$38,0),MATCH(F$2,'Master Emp List'!$A$1:$I$1,0))</f>
+        <v>9.9499999999999993</v>
+      </c>
       <c r="G9" s="68"/>
     </row>
     <row r="10" spans="2:7">
@@ -11620,47 +11686,83 @@
         <v>1284</v>
       </c>
       <c r="C10" s="11" t="str">
-        <f>IFERROR(VLOOKUP($B10,'Master Emp List'!$A$1:$I$38,3,FALSE), "EMP ID NOT FOUND")</f>
+        <f>INDEX('Master Emp List'!$A$1:$I$38,MATCH($B10,'Master Emp List'!$A$1:$A$38,0),MATCH(C$2,'Master Emp List'!$A$1:$I$1,0))</f>
         <v>Frank</v>
       </c>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
+      <c r="D10" s="11" t="str">
+        <f>INDEX('Master Emp List'!$A$1:$I$38,MATCH($B10,'Master Emp List'!$A$1:$A$38,0),MATCH(D$2,'Master Emp List'!$A$1:$I$1,0))</f>
+        <v>Bellwood</v>
+      </c>
+      <c r="E10" s="11" t="str">
+        <f>INDEX('Master Emp List'!$A$1:$I$38,MATCH($B10,'Master Emp List'!$A$1:$A$38,0),MATCH(E$2,'Master Emp List'!$A$1:$I$1,0))</f>
+        <v>MK</v>
+      </c>
+      <c r="F10" s="11">
+        <f>INDEX('Master Emp List'!$A$1:$I$38,MATCH($B10,'Master Emp List'!$A$1:$A$38,0),MATCH(F$2,'Master Emp List'!$A$1:$I$1,0))</f>
+        <v>12.3</v>
+      </c>
       <c r="G10" s="68"/>
     </row>
     <row r="11" spans="2:7">
       <c r="B11" s="10">
         <v>0</v>
       </c>
-      <c r="C11" s="11" t="str">
-        <f>IFERROR(VLOOKUP($B11,'Master Emp List'!$A$1:$I$38,3,FALSE), "EMP ID NOT FOUND")</f>
-        <v>EMP ID NOT FOUND</v>
-      </c>
-      <c r="D11" s="11"/>
-      <c r="E11" s="11"/>
-      <c r="F11" s="11"/>
+      <c r="C11" s="11" t="e">
+        <f>INDEX('Master Emp List'!$A$1:$I$38,MATCH($B11,'Master Emp List'!$A$1:$A$38,0),MATCH(C$2,'Master Emp List'!$A$1:$I$1,0))</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D11" s="11" t="e">
+        <f>INDEX('Master Emp List'!$A$1:$I$38,MATCH($B11,'Master Emp List'!$A$1:$A$38,0),MATCH(D$2,'Master Emp List'!$A$1:$I$1,0))</f>
+        <v>#N/A</v>
+      </c>
+      <c r="E11" s="11" t="e">
+        <f>INDEX('Master Emp List'!$A$1:$I$38,MATCH($B11,'Master Emp List'!$A$1:$A$38,0),MATCH(E$2,'Master Emp List'!$A$1:$I$1,0))</f>
+        <v>#N/A</v>
+      </c>
+      <c r="F11" s="11" t="e">
+        <f>INDEX('Master Emp List'!$A$1:$I$38,MATCH($B11,'Master Emp List'!$A$1:$A$38,0),MATCH(F$2,'Master Emp List'!$A$1:$I$1,0))</f>
+        <v>#N/A</v>
+      </c>
       <c r="G11" s="68"/>
     </row>
     <row r="12" spans="2:7">
       <c r="B12" s="10"/>
-      <c r="C12" s="11" t="str">
-        <f>IFERROR(VLOOKUP($B12,'Master Emp List'!$A$1:$I$38,3,FALSE), "EMP ID NOT FOUND")</f>
-        <v>EMP ID NOT FOUND</v>
-      </c>
-      <c r="D12" s="11"/>
-      <c r="E12" s="11"/>
-      <c r="F12" s="11"/>
+      <c r="C12" s="11" t="e">
+        <f>INDEX('Master Emp List'!$A$1:$I$38,MATCH($B12,'Master Emp List'!$A$1:$A$38,0),MATCH(C$2,'Master Emp List'!$A$1:$I$1,0))</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D12" s="11" t="e">
+        <f>INDEX('Master Emp List'!$A$1:$I$38,MATCH($B12,'Master Emp List'!$A$1:$A$38,0),MATCH(D$2,'Master Emp List'!$A$1:$I$1,0))</f>
+        <v>#N/A</v>
+      </c>
+      <c r="E12" s="11" t="e">
+        <f>INDEX('Master Emp List'!$A$1:$I$38,MATCH($B12,'Master Emp List'!$A$1:$A$38,0),MATCH(E$2,'Master Emp List'!$A$1:$I$1,0))</f>
+        <v>#N/A</v>
+      </c>
+      <c r="F12" s="11" t="e">
+        <f>INDEX('Master Emp List'!$A$1:$I$38,MATCH($B12,'Master Emp List'!$A$1:$A$38,0),MATCH(F$2,'Master Emp List'!$A$1:$I$1,0))</f>
+        <v>#N/A</v>
+      </c>
       <c r="G12" s="68"/>
     </row>
     <row r="13" spans="2:7">
       <c r="B13" s="10"/>
-      <c r="C13" s="11" t="str">
-        <f>IFERROR(VLOOKUP($B13,'Master Emp List'!$A$1:$I$38,3,FALSE), "EMP ID NOT FOUND")</f>
-        <v>EMP ID NOT FOUND</v>
-      </c>
-      <c r="D13" s="11"/>
-      <c r="E13" s="11"/>
-      <c r="F13" s="11"/>
+      <c r="C13" s="11" t="e">
+        <f>INDEX('Master Emp List'!$A$1:$I$38,MATCH($B13,'Master Emp List'!$A$1:$A$38,0),MATCH(C$2,'Master Emp List'!$A$1:$I$1,0))</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D13" s="11" t="e">
+        <f>INDEX('Master Emp List'!$A$1:$I$38,MATCH($B13,'Master Emp List'!$A$1:$A$38,0),MATCH(D$2,'Master Emp List'!$A$1:$I$1,0))</f>
+        <v>#N/A</v>
+      </c>
+      <c r="E13" s="11" t="e">
+        <f>INDEX('Master Emp List'!$A$1:$I$38,MATCH($B13,'Master Emp List'!$A$1:$A$38,0),MATCH(E$2,'Master Emp List'!$A$1:$I$1,0))</f>
+        <v>#N/A</v>
+      </c>
+      <c r="F13" s="11" t="e">
+        <f>INDEX('Master Emp List'!$A$1:$I$38,MATCH($B13,'Master Emp List'!$A$1:$A$38,0),MATCH(F$2,'Master Emp List'!$A$1:$I$1,0))</f>
+        <v>#N/A</v>
+      </c>
       <c r="G13" s="68"/>
     </row>
     <row r="14" spans="2:7">
@@ -11668,12 +11770,21 @@
         <v>1302</v>
       </c>
       <c r="C14" s="11" t="str">
-        <f>IFERROR(VLOOKUP($B14,'Master Emp List'!$A$1:$I$38,3,FALSE), "EMP ID NOT FOUND")</f>
+        <f>INDEX('Master Emp List'!$A$1:$I$38,MATCH($B14,'Master Emp List'!$A$1:$A$38,0),MATCH(C$2,'Master Emp List'!$A$1:$I$1,0))</f>
         <v>Randy</v>
       </c>
-      <c r="D14" s="11"/>
-      <c r="E14" s="11"/>
-      <c r="F14" s="11"/>
+      <c r="D14" s="11" t="str">
+        <f>INDEX('Master Emp List'!$A$1:$I$38,MATCH($B14,'Master Emp List'!$A$1:$A$38,0),MATCH(D$2,'Master Emp List'!$A$1:$I$1,0))</f>
+        <v>Sindole</v>
+      </c>
+      <c r="E14" s="11" t="str">
+        <f>INDEX('Master Emp List'!$A$1:$I$38,MATCH($B14,'Master Emp List'!$A$1:$A$38,0),MATCH(E$2,'Master Emp List'!$A$1:$I$1,0))</f>
+        <v>MK</v>
+      </c>
+      <c r="F14" s="11">
+        <f>INDEX('Master Emp List'!$A$1:$I$38,MATCH($B14,'Master Emp List'!$A$1:$A$38,0),MATCH(F$2,'Master Emp List'!$A$1:$I$1,0))</f>
+        <v>14.25</v>
+      </c>
       <c r="G14" s="68"/>
     </row>
     <row r="15" spans="2:7">
@@ -11681,12 +11792,21 @@
         <v>1310</v>
       </c>
       <c r="C15" s="11" t="str">
-        <f>IFERROR(VLOOKUP($B15,'Master Emp List'!$A$1:$I$38,3,FALSE), "EMP ID NOT FOUND")</f>
+        <f>INDEX('Master Emp List'!$A$1:$I$38,MATCH($B15,'Master Emp List'!$A$1:$A$38,0),MATCH(C$2,'Master Emp List'!$A$1:$I$1,0))</f>
         <v>Ellen</v>
       </c>
-      <c r="D15" s="11"/>
-      <c r="E15" s="11"/>
-      <c r="F15" s="11"/>
+      <c r="D15" s="11" t="str">
+        <f>INDEX('Master Emp List'!$A$1:$I$38,MATCH($B15,'Master Emp List'!$A$1:$A$38,0),MATCH(D$2,'Master Emp List'!$A$1:$I$1,0))</f>
+        <v>Smith</v>
+      </c>
+      <c r="E15" s="11" t="str">
+        <f>INDEX('Master Emp List'!$A$1:$I$38,MATCH($B15,'Master Emp List'!$A$1:$A$38,0),MATCH(E$2,'Master Emp List'!$A$1:$I$1,0))</f>
+        <v>MF</v>
+      </c>
+      <c r="F15" s="11">
+        <f>INDEX('Master Emp List'!$A$1:$I$38,MATCH($B15,'Master Emp List'!$A$1:$A$38,0),MATCH(F$2,'Master Emp List'!$A$1:$I$1,0))</f>
+        <v>11.5</v>
+      </c>
       <c r="G15" s="68"/>
     </row>
     <row r="16" spans="2:7">
@@ -11694,12 +11814,21 @@
         <v>1329</v>
       </c>
       <c r="C16" s="11" t="str">
-        <f>IFERROR(VLOOKUP($B16,'Master Emp List'!$A$1:$I$38,3,FALSE), "EMP ID NOT FOUND")</f>
+        <f>INDEX('Master Emp List'!$A$1:$I$38,MATCH($B16,'Master Emp List'!$A$1:$A$38,0),MATCH(C$2,'Master Emp List'!$A$1:$I$1,0))</f>
         <v>Tuome</v>
       </c>
-      <c r="D16" s="11"/>
-      <c r="E16" s="11"/>
-      <c r="F16" s="11"/>
+      <c r="D16" s="11" t="str">
+        <f>INDEX('Master Emp List'!$A$1:$I$38,MATCH($B16,'Master Emp List'!$A$1:$A$38,0),MATCH(D$2,'Master Emp List'!$A$1:$I$1,0))</f>
+        <v>Vuanuo</v>
+      </c>
+      <c r="E16" s="11" t="str">
+        <f>INDEX('Master Emp List'!$A$1:$I$38,MATCH($B16,'Master Emp List'!$A$1:$A$38,0),MATCH(E$2,'Master Emp List'!$A$1:$I$1,0))</f>
+        <v>AC</v>
+      </c>
+      <c r="F16" s="11">
+        <f>INDEX('Master Emp List'!$A$1:$I$38,MATCH($B16,'Master Emp List'!$A$1:$A$38,0),MATCH(F$2,'Master Emp List'!$A$1:$I$1,0))</f>
+        <v>10.35</v>
+      </c>
       <c r="G16" s="68"/>
     </row>
     <row r="17" spans="2:7">
@@ -11707,25 +11836,43 @@
         <v>1333</v>
       </c>
       <c r="C17" s="11" t="str">
-        <f>IFERROR(VLOOKUP($B17,'Master Emp List'!$A$1:$I$38,3,FALSE), "EMP ID NOT FOUND")</f>
+        <f>INDEX('Master Emp List'!$A$1:$I$38,MATCH($B17,'Master Emp List'!$A$1:$A$38,0),MATCH(C$2,'Master Emp List'!$A$1:$I$1,0))</f>
         <v>Tadeuz</v>
       </c>
-      <c r="D17" s="11"/>
-      <c r="E17" s="11"/>
-      <c r="F17" s="11"/>
+      <c r="D17" s="11" t="str">
+        <f>INDEX('Master Emp List'!$A$1:$I$38,MATCH($B17,'Master Emp List'!$A$1:$A$38,0),MATCH(D$2,'Master Emp List'!$A$1:$I$1,0))</f>
+        <v>Szcznyck</v>
+      </c>
+      <c r="E17" s="11" t="str">
+        <f>INDEX('Master Emp List'!$A$1:$I$38,MATCH($B17,'Master Emp List'!$A$1:$A$38,0),MATCH(E$2,'Master Emp List'!$A$1:$I$1,0))</f>
+        <v>HR</v>
+      </c>
+      <c r="F17" s="11">
+        <f>INDEX('Master Emp List'!$A$1:$I$38,MATCH($B17,'Master Emp List'!$A$1:$A$38,0),MATCH(F$2,'Master Emp List'!$A$1:$I$1,0))</f>
+        <v>10.15</v>
+      </c>
       <c r="G17" s="68"/>
     </row>
-    <row r="18" spans="2:7" ht="13.8" thickBot="1">
+    <row r="18" spans="2:7" ht="13" thickBot="1">
       <c r="B18" s="13">
         <v>1368</v>
       </c>
       <c r="C18" s="11" t="str">
-        <f>IFERROR(VLOOKUP($B18,'Master Emp List'!$A$1:$I$38,3,FALSE), "EMP ID NOT FOUND")</f>
+        <f>INDEX('Master Emp List'!$A$1:$I$38,MATCH($B18,'Master Emp List'!$A$1:$A$38,0),MATCH(C$2,'Master Emp List'!$A$1:$I$1,0))</f>
         <v>Tammy</v>
       </c>
-      <c r="D18" s="11"/>
-      <c r="E18" s="11"/>
-      <c r="F18" s="11"/>
+      <c r="D18" s="11" t="str">
+        <f>INDEX('Master Emp List'!$A$1:$I$38,MATCH($B18,'Master Emp List'!$A$1:$A$38,0),MATCH(D$2,'Master Emp List'!$A$1:$I$1,0))</f>
+        <v>Wu</v>
+      </c>
+      <c r="E18" s="11" t="str">
+        <f>INDEX('Master Emp List'!$A$1:$I$38,MATCH($B18,'Master Emp List'!$A$1:$A$38,0),MATCH(E$2,'Master Emp List'!$A$1:$I$1,0))</f>
+        <v>AD</v>
+      </c>
+      <c r="F18" s="11">
+        <f>INDEX('Master Emp List'!$A$1:$I$38,MATCH($B18,'Master Emp List'!$A$1:$A$38,0),MATCH(F$2,'Master Emp List'!$A$1:$I$1,0))</f>
+        <v>12.25</v>
+      </c>
       <c r="G18" s="68"/>
     </row>
   </sheetData>
@@ -11745,8 +11892,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" customHeight="1"/>
   <cols>
-    <col min="1" max="8" width="14.109375" style="6" customWidth="1"/>
-    <col min="9" max="9" width="14.109375" customWidth="1"/>
+    <col min="1" max="8" width="14.08984375" style="6" customWidth="1"/>
+    <col min="9" max="9" width="14.08984375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="24.75" customHeight="1">
@@ -12863,30 +13010,30 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="12.5"/>
   <cols>
-    <col min="1" max="1" width="30.109375" style="56" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.6640625" style="56" customWidth="1"/>
-    <col min="3" max="3" width="16.88671875" style="56" customWidth="1"/>
-    <col min="4" max="4" width="8.109375" style="56" customWidth="1"/>
-    <col min="5" max="5" width="7.33203125" style="56" customWidth="1"/>
-    <col min="6" max="6" width="10.5546875" style="56" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.6640625" style="56" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.109375" style="56"/>
+    <col min="1" max="1" width="30.08984375" style="56" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.6328125" style="56" customWidth="1"/>
+    <col min="3" max="3" width="16.90625" style="56" customWidth="1"/>
+    <col min="4" max="4" width="8.08984375" style="56" customWidth="1"/>
+    <col min="5" max="5" width="7.36328125" style="56" customWidth="1"/>
+    <col min="6" max="6" width="10.54296875" style="56" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.6328125" style="56" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.08984375" style="56"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="13.8" thickBot="1"/>
+    <row r="1" spans="1:2" ht="13" thickBot="1"/>
     <row r="2" spans="1:2" ht="22.5" customHeight="1" thickBot="1">
       <c r="A2" s="130" t="s">
         <v>231</v>
       </c>
       <c r="B2" s="131"/>
     </row>
-    <row r="3" spans="1:2" ht="16.8" thickTop="1" thickBot="1">
+    <row r="3" spans="1:2" ht="16.5" thickTop="1" thickBot="1">
       <c r="A3" s="62" t="s">
         <v>230</v>
       </c>
@@ -12898,7 +13045,7 @@
       <c r="A4" s="60"/>
       <c r="B4" s="59"/>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" ht="13">
       <c r="A5" s="63" t="s">
         <v>229</v>
       </c>
@@ -12907,17 +13054,23 @@
         <v>150</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" ht="13">
       <c r="A6" s="63" t="s">
         <v>228</v>
       </c>
-      <c r="B6" s="58"/>
-    </row>
-    <row r="7" spans="1:2" ht="13.8" thickBot="1">
+      <c r="B6" s="58">
+        <f>HLOOKUP($B$3,'Master Inventory List'!$A$2:$G$5,3,FALSE)</f>
+        <v>110</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="13.5" thickBot="1">
       <c r="A7" s="64" t="s">
         <v>227</v>
       </c>
-      <c r="B7" s="58"/>
+      <c r="B7" s="58">
+        <f>HLOOKUP($B$3,'Master Inventory List'!$A$2:$G$5,4,FALSE)</f>
+        <v>115</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -12937,13 +13090,13 @@
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="12.5"/>
   <cols>
-    <col min="1" max="1" width="14.88671875" style="56" customWidth="1"/>
-    <col min="2" max="16384" width="9.109375" style="56"/>
+    <col min="1" max="1" width="14.90625" style="56" customWidth="1"/>
+    <col min="2" max="16384" width="9.08984375" style="56"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" ht="13">
       <c r="A2" s="65" t="s">
         <v>238</v>
       </c>
@@ -12966,7 +13119,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" ht="13">
       <c r="A3" s="67" t="s">
         <v>234</v>
       </c>
@@ -12989,7 +13142,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" ht="13">
       <c r="A4" s="67" t="s">
         <v>233</v>
       </c>
@@ -13012,7 +13165,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" ht="13">
       <c r="A5" s="67" t="s">
         <v>232</v>
       </c>
@@ -13049,14 +13202,14 @@
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultRowHeight="12.5"/>
   <cols>
-    <col min="1" max="1" width="3.109375" customWidth="1"/>
+    <col min="1" max="1" width="3.08984375" customWidth="1"/>
     <col min="2" max="2" width="10" customWidth="1"/>
     <col min="3" max="3" width="16" customWidth="1"/>
     <col min="4" max="4" width="19" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.109375" customWidth="1"/>
-    <col min="6" max="6" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.08984375" customWidth="1"/>
+    <col min="6" max="6" width="18.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:6" ht="41.25" customHeight="1" thickBot="1">
@@ -13067,7 +13220,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="3" spans="2:6" ht="13.8">
+    <row r="3" spans="2:6" ht="14">
       <c r="B3" s="120" t="s">
         <v>283</v>
       </c>
@@ -13195,8 +13348,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" customHeight="1"/>
   <cols>
-    <col min="1" max="8" width="14.109375" style="6" customWidth="1"/>
-    <col min="9" max="9" width="14.109375" customWidth="1"/>
+    <col min="1" max="8" width="14.08984375" style="6" customWidth="1"/>
+    <col min="9" max="9" width="14.08984375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="24.75" customHeight="1">
@@ -14318,19 +14471,19 @@
       <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultRowHeight="12.5"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" customWidth="1"/>
-    <col min="2" max="2" width="27.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.5546875" customWidth="1"/>
-    <col min="4" max="4" width="3.109375" customWidth="1"/>
-    <col min="5" max="5" width="11.88671875" customWidth="1"/>
-    <col min="6" max="6" width="10.5546875" customWidth="1"/>
-    <col min="7" max="7" width="14.5546875" customWidth="1"/>
-    <col min="8" max="8" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.453125" customWidth="1"/>
+    <col min="2" max="2" width="27.90625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.54296875" customWidth="1"/>
+    <col min="4" max="4" width="3.08984375" customWidth="1"/>
+    <col min="5" max="5" width="11.90625" customWidth="1"/>
+    <col min="6" max="6" width="10.54296875" customWidth="1"/>
+    <col min="7" max="7" width="14.54296875" customWidth="1"/>
+    <col min="8" max="8" width="10.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" ht="13">
       <c r="A2" s="35" t="s">
         <v>168</v>
       </c>
@@ -14354,7 +14507,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" ht="13">
       <c r="A3" s="22" t="s">
         <v>169</v>
       </c>
@@ -14378,7 +14531,7 @@
         <v>WW</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" ht="13">
       <c r="A4" s="22" t="s">
         <v>170</v>
       </c>
@@ -14393,7 +14546,7 @@
       <c r="F4" s="17"/>
       <c r="G4" s="17"/>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" ht="13">
       <c r="A5" s="22" t="s">
         <v>171</v>
       </c>
@@ -14408,7 +14561,7 @@
       <c r="F5" s="17"/>
       <c r="G5" s="17"/>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" ht="13">
       <c r="A6" s="22" t="s">
         <v>172</v>
       </c>
@@ -14423,7 +14576,7 @@
       <c r="F6" s="17"/>
       <c r="G6" s="17"/>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" ht="13">
       <c r="A7" s="22" t="s">
         <v>173</v>
       </c>
@@ -14438,7 +14591,7 @@
       <c r="F7" s="17"/>
       <c r="G7" s="17"/>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" ht="13">
       <c r="A8" s="22" t="s">
         <v>174</v>
       </c>
@@ -14453,7 +14606,7 @@
       <c r="F8" s="17"/>
       <c r="G8" s="17"/>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" ht="13">
       <c r="A9" s="22" t="s">
         <v>175</v>
       </c>
@@ -14468,7 +14621,7 @@
       <c r="F9" s="17"/>
       <c r="G9" s="17"/>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" ht="13">
       <c r="A10" s="22" t="s">
         <v>176</v>
       </c>
@@ -14483,7 +14636,7 @@
       <c r="F10" s="17"/>
       <c r="G10" s="17"/>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" ht="13">
       <c r="A11" s="22" t="s">
         <v>177</v>
       </c>
@@ -14498,7 +14651,7 @@
       <c r="F11" s="17"/>
       <c r="G11" s="17"/>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" ht="13">
       <c r="A12" s="22" t="s">
         <v>204</v>
       </c>
@@ -14513,7 +14666,7 @@
       <c r="F12" s="17"/>
       <c r="G12" s="17"/>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" ht="13">
       <c r="A13" s="22" t="s">
         <v>205</v>
       </c>
@@ -14528,7 +14681,7 @@
       <c r="F13" s="17"/>
       <c r="G13" s="17"/>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" ht="13">
       <c r="A14" s="22" t="s">
         <v>206</v>
       </c>
@@ -14543,7 +14696,7 @@
       <c r="F14" s="17"/>
       <c r="G14" s="17"/>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" ht="13">
       <c r="A15" s="22" t="s">
         <v>207</v>
       </c>
@@ -14558,7 +14711,7 @@
       <c r="F15" s="17"/>
       <c r="G15" s="17"/>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" ht="13">
       <c r="A16" s="22" t="s">
         <v>208</v>
       </c>
@@ -14573,7 +14726,7 @@
       <c r="F16" s="17"/>
       <c r="G16" s="17"/>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" ht="13">
       <c r="A17" s="22" t="s">
         <v>209</v>
       </c>
@@ -14588,7 +14741,7 @@
       <c r="F17" s="17"/>
       <c r="G17" s="17"/>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:7" ht="13">
       <c r="A18" s="22" t="s">
         <v>210</v>
       </c>
@@ -14603,7 +14756,7 @@
       <c r="F18" s="17"/>
       <c r="G18" s="17"/>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:7" ht="13">
       <c r="A19" s="22" t="s">
         <v>178</v>
       </c>
@@ -14618,7 +14771,7 @@
       <c r="F19" s="17"/>
       <c r="G19" s="17"/>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:7" ht="13">
       <c r="A20" s="22" t="s">
         <v>211</v>
       </c>
@@ -14633,7 +14786,7 @@
       <c r="F20" s="17"/>
       <c r="G20" s="17"/>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:7" ht="13">
       <c r="A21" s="22" t="s">
         <v>212</v>
       </c>
@@ -14648,7 +14801,7 @@
       <c r="F21" s="17"/>
       <c r="G21" s="17"/>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:7" ht="13">
       <c r="A22" s="22" t="s">
         <v>217</v>
       </c>
@@ -14663,7 +14816,7 @@
       <c r="F22" s="17"/>
       <c r="G22" s="17"/>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:7" ht="13">
       <c r="A23" s="22" t="s">
         <v>218</v>
       </c>
@@ -14678,7 +14831,7 @@
       <c r="F23" s="17"/>
       <c r="G23" s="17"/>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="1:7" ht="13">
       <c r="A24" s="22" t="s">
         <v>214</v>
       </c>
@@ -14693,7 +14846,7 @@
       <c r="F24" s="17"/>
       <c r="G24" s="17"/>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="1:7" ht="13">
       <c r="A25" s="22" t="s">
         <v>215</v>
       </c>
@@ -14708,7 +14861,7 @@
       <c r="F25" s="17"/>
       <c r="G25" s="17"/>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26" spans="1:7" ht="13">
       <c r="A26" s="22" t="s">
         <v>216</v>
       </c>

</xml_diff>